<commit_message>
Correcting investment:  INVEST IN NEXT ROUNDS PORISTIVE NPVS
</commit_message>
<xml_diff>
--- a/emlabpy/test_npv.xlsx
+++ b/emlabpy/test_npv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\emlabpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DDB572-A2E6-4495-AA3B-6F8CBABFED35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E878F66-8C50-4332-A3BF-8E935D218D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2DEE18F0-ABF9-4F99-8667-5A8B8B4F2408}"/>
+    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2DEE18F0-ABF9-4F99-8667-5A8B8B4F2408}"/>
   </bookViews>
   <sheets>
     <sheet name="solar 150MW" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
   <si>
     <t>technology</t>
   </si>
@@ -106,9 +106,6 @@
     <t>future value</t>
   </si>
   <si>
-    <t>Annuity python</t>
-  </si>
-  <si>
     <t>yearly income annuity</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">difference </t>
+  </si>
+  <si>
+    <t>debtinterestRate</t>
   </si>
 </sst>
 </file>
@@ -928,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B907B72A-41D5-4B21-A796-455CB3645BCE}">
-  <dimension ref="B1:V29"/>
+  <dimension ref="B1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -939,6 +939,7 @@
     <col min="2" max="2" width="32.6328125" customWidth="1"/>
     <col min="3" max="3" width="27.26953125" customWidth="1"/>
     <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22">
@@ -951,10 +952,10 @@
     </row>
     <row r="2" spans="2:22">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="3" spans="2:22">
@@ -962,7 +963,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="2:22">
@@ -971,7 +972,7 @@
       </c>
       <c r="C4">
         <f>((1-C5)*C3)+(C5*C2)</f>
-        <v>0.1</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="5" spans="2:22">
@@ -987,8 +988,8 @@
         <v>7</v>
       </c>
       <c r="C6" s="5">
-        <f>832316.88*150</f>
-        <v>124847532</v>
+        <f>832316.88*10</f>
+        <v>8323168.7999999998</v>
       </c>
     </row>
     <row r="7" spans="2:22">
@@ -1043,178 +1044,101 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
-        <f>C9*(C5)/C11</f>
-        <v>1995000</v>
+      <c r="C12" s="6">
+        <f>-C9*(C5)/C11</f>
+        <v>-1995000</v>
       </c>
     </row>
     <row r="13" spans="2:22">
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <f>C6-C12-C7</f>
-        <v>121765032</v>
+        <v>19</v>
+      </c>
+      <c r="C13" s="6">
+        <f>PMT(C2,C11,(C9*C5),0,0)</f>
+        <v>-3766277.7371559022</v>
       </c>
     </row>
     <row r="14" spans="2:22">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6">
-        <f>C6+C22-C7</f>
-        <v>119073392.97157542</v>
+        <f>C6+C12-C7</f>
+        <v>5240668.8</v>
       </c>
     </row>
     <row r="15" spans="2:22">
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6">
+        <f>C6+C13-C7</f>
+        <v>3469391.0628440976</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22">
+      <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>4</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>5</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>6</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>7</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>8</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>9</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>10</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>11</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>12</v>
       </c>
-      <c r="O15">
+      <c r="O16">
         <v>13</v>
       </c>
-      <c r="P15">
+      <c r="P16">
         <v>14</v>
       </c>
-      <c r="Q15">
+      <c r="Q16">
         <v>15</v>
       </c>
-      <c r="R15">
+      <c r="R16">
         <v>16</v>
       </c>
-      <c r="S15">
+      <c r="S16">
         <v>17</v>
       </c>
-      <c r="T15">
+      <c r="T16">
         <v>18</v>
       </c>
-      <c r="U15">
+      <c r="U16">
         <v>19</v>
       </c>
-      <c r="V15">
+      <c r="V16">
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22">
-      <c r="B16">
-        <f>-(1-C5)*C9</f>
-        <v>-17100000.000000004</v>
-      </c>
-      <c r="C16">
-        <f>C13</f>
-        <v>121765032</v>
-      </c>
-      <c r="D16">
-        <f>C16</f>
-        <v>121765032</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ref="E16:V17" si="0">D16</f>
-        <v>121765032</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="0"/>
-        <v>121765032</v>
       </c>
     </row>
     <row r="17" spans="2:22">
@@ -1222,151 +1146,220 @@
         <f>-(1-C5)*C9</f>
         <v>-17100000.000000004</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17">
         <f>C14</f>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="D17" s="6">
+        <v>5240668.8</v>
+      </c>
+      <c r="D17">
         <f>C17</f>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="E17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="F17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="G17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="H17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="I17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="J17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="K17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="L17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="M17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="N17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="O17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="P17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="Q17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="R17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="S17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="T17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="U17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
-      </c>
-      <c r="V17" s="6">
-        <f t="shared" si="0"/>
-        <v>119073392.97157542</v>
+        <v>5240668.8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:V18" si="0">D17</f>
+        <v>5240668.8</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="0"/>
+        <v>5240668.8</v>
       </c>
     </row>
     <row r="18" spans="2:22">
-      <c r="B18" t="s">
-        <v>20</v>
+      <c r="B18">
+        <f>-(1-C5)*C9</f>
+        <v>-17100000.000000004</v>
+      </c>
+      <c r="C18" s="6">
+        <f>C15</f>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="D18" s="6">
+        <f>C18</f>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="0"/>
+        <v>3469391.0628440976</v>
       </c>
     </row>
     <row r="19" spans="2:22">
       <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:22">
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="6">
-        <f>PMT(C2,C11,(C9*C5),0,0)</f>
-        <v>-4686639.0284245769</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22">
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="6">
-        <v>-4686639.0284245797</v>
-      </c>
-    </row>
     <row r="24" spans="2:22">
-      <c r="C24" s="3">
-        <f>C22-C23</f>
-        <v>0</v>
-      </c>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="2:22">
-      <c r="C25" s="7"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="2:22">
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="3">
-        <f>NPV(C4,B16:U16)</f>
-        <v>910413420.58862174</v>
-      </c>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="2:22">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" s="3">
         <f>NPV(C4,B17:U17)</f>
-        <v>889944924.78083479</v>
-      </c>
-    </row>
-    <row r="29" spans="2:22">
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="8">
-        <f>(C26-C27)/C27</f>
-        <v>2.2999733172058577E-2</v>
+        <v>29003734.746643025</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3">
+        <f>NPV(C4,B18:U18)</f>
+        <v>13874051.33785782</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="8">
+        <f>(C27-C28)/C28</f>
+        <v>1.0905021929320076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>